<commit_message>
updating set up template
</commit_message>
<xml_diff>
--- a/Projects/GSKJP/Data/gsk_set_up.xlsx
+++ b/Projects/GSKJP/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -65,6 +65,9 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
+    <t xml:space="preserve">Oral Main Shelf</t>
+  </si>
+  <si>
     <t xml:space="preserve">Include </t>
   </si>
   <si>
@@ -74,7 +77,13 @@
     <t xml:space="preserve">Oral Care</t>
   </si>
   <si>
+    <t xml:space="preserve">Tooth paste,Denture cleanser,Denture adhesive</t>
+  </si>
+  <si>
     <t xml:space="preserve">Linear SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exclude</t>
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
@@ -87,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,6 +133,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -188,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,12 +232,24 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -297,7 +324,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -315,21 +342,21 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" activeCellId="0" sqref="J2:J3"/>
+      <selection pane="bottomRight" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="1013" min="12" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1014" style="0" width="8.78542510121457"/>
   </cols>
@@ -380,30 +407,34 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="ALZ2" s="0"/>
       <c r="AMA2" s="0"/>
       <c r="AMB2" s="0"/>
@@ -416,42 +447,54 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="9"/>
+      <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
gskjp phase b calculation
</commit_message>
<xml_diff>
--- a/Projects/GSKJP/Data/gsk_set_up.xlsx
+++ b/Projects/GSKJP/Data/gsk_set_up.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toughgrip,Polident,Poligrip</t>
   </si>
   <si>
     <t xml:space="preserve">GSK_PLN_BLOCK_SCORE</t>
@@ -99,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -136,6 +139,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -200,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,6 +244,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -327,21 +340,22 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.78542510121457"/>
   </cols>
@@ -467,20 +481,32 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="8"/>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added col: Location type in the gsk_set_up.xlsx template to align with the global template change[sdk_factory 07e08dc9b83903ea0a6d25b43402819b737c1df6]. Also to avoid code-crash if this change is deployed in the near future for gskjp
</commit_message>
<xml_diff>
--- a/Projects/GSKJP/Data/gsk_set_up.xlsx
+++ b/Projects/GSKJP/Data/gsk_set_up.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">Include POSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location type</t>
   </si>
   <si>
     <t xml:space="preserve">Linear SOS</t>
@@ -129,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -158,6 +161,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibre"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -236,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,7 +264,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,12 +302,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -371,14 +386,14 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.39"/>
@@ -390,11 +405,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="43.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="12" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="14" style="1" width="8.79"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -431,7 +447,9 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AMA1" s="0"/>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
@@ -442,37 +460,37 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="8" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="9" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AMA2" s="0"/>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="7"/>
       <c r="AMB2" s="0"/>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
@@ -483,179 +501,185 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="8"/>
-      <c r="J8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="L8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>